<commit_message>
Signed-off-by: mahmouddgamall <mahmouddgamall93@gmail.com>Updating SRS
</commit_message>
<xml_diff>
--- a/Software Specification/SRS/Review.xlsx
+++ b/Software Specification/SRS/Review.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41A97F0E-1AEF-4476-B67D-D51C8A5B236F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CYRS" sheetId="5" r:id="rId1"/>
@@ -17,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="21">
   <si>
     <t>Review point</t>
   </si>
@@ -96,12 +97,15 @@
   <si>
     <t>Add also HIS in the reference table</t>
   </si>
+  <si>
+    <t>Accepted</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,7 +169,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="42">
+  <dxfs count="20">
     <dxf>
       <font>
         <condense val="0"/>
@@ -232,6 +236,13 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -242,16 +253,7 @@
     </dxf>
     <dxf>
       <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
+        <color rgb="FFFF0000"/>
       </font>
     </dxf>
     <dxf>
@@ -268,7 +270,9 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FFFF0000"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
       </font>
     </dxf>
     <dxf>
@@ -338,199 +342,16 @@
         <color rgb="FFFF0000"/>
       </font>
     </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -577,7 +398,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -609,9 +430,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -643,6 +482,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -818,14 +675,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="53.5703125" style="5" customWidth="1"/>
@@ -834,7 +691,7 @@
     <col min="6" max="6" width="41.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -854,7 +711,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30">
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>43984</v>
       </c>
@@ -864,12 +721,14 @@
       <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="4"/>
+      <c r="D2" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="30">
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>43984</v>
       </c>
@@ -879,12 +738,14 @@
       <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="30">
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>43984</v>
       </c>
@@ -894,12 +755,14 @@
       <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="4"/>
+      <c r="D4" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="E4" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="30">
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>43984</v>
       </c>
@@ -909,12 +772,14 @@
       <c r="C5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="E5" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="30">
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>43984</v>
       </c>
@@ -924,12 +789,14 @@
       <c r="C6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="4"/>
+      <c r="D6" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="E6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="60">
+    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>43984</v>
       </c>
@@ -939,12 +806,14 @@
       <c r="C7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="4"/>
+      <c r="D7" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="E7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="30">
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>43984</v>
       </c>
@@ -954,12 +823,14 @@
       <c r="C8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="4"/>
+      <c r="D8" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="E8" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="45">
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>43984</v>
       </c>
@@ -969,12 +840,14 @@
       <c r="C9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="4"/>
+      <c r="D9" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="E9" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="30">
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>43984</v>
       </c>
@@ -984,12 +857,14 @@
       <c r="C10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="4"/>
+      <c r="D10" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="E10" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="45">
+    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>43984</v>
       </c>
@@ -999,12 +874,14 @@
       <c r="C11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="4"/>
+      <c r="D11" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="E11" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="150">
+    <row r="12" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>43984</v>
       </c>
@@ -1014,12 +891,14 @@
       <c r="C12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="4"/>
+      <c r="D12" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="E12" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>43984</v>
       </c>
@@ -1029,93 +908,95 @@
       <c r="C13" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="4"/>
+      <c r="D13" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="E13" s="1" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2">
-    <cfRule type="containsText" dxfId="29" priority="48" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="19" priority="48" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="49" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="18" priority="49" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="50" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="17" priority="50" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="26" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="46" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="47" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="containsText" dxfId="24" priority="13" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="14" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="15" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="21" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="containsText" dxfId="19" priority="8" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="9" priority="8" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="9" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="10" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="7" priority="10" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5:E13">
-    <cfRule type="containsText" dxfId="14" priority="3" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="4" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="5" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D13">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D13" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Accepted, Rejected"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E13" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Open, Closed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>